<commit_message>
Used the serializable dictionary instead of list to store skill config
</commit_message>
<xml_diff>
--- a/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/__tables__.xlsx
+++ b/Unity/NewWheel/VampireBuilder1/DesignerConfigs/Datas/__tables__.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\GobangAdventure\Unity\NewWheel\VampireBuilder1\DesignData\Datas\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\GobangAdventure\Unity\NewWheel\VampireBuilder1\DesignerConfigs\Datas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40E5E0B0-9CEF-4926-A2A2-DE5C4DD6C635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CB05C0C-084B-421E-8C82-88E9C059C289}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="3675" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="1215" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -131,17 +131,17 @@
     <t>skill.xlsx</t>
   </si>
   <si>
-    <t>skill.TbSkill</t>
-  </si>
-  <si>
     <t>Skill</t>
+  </si>
+  <si>
+    <t>TbSkillConfig</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -151,9 +151,16 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -184,15 +191,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -474,7 +484,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -590,11 +600,11 @@
       </c>
     </row>
     <row r="4" spans="1:13">
-      <c r="B4" t="s">
+      <c r="B4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" t="s">
         <v>32</v>
-      </c>
-      <c r="C4" t="s">
-        <v>33</v>
       </c>
       <c r="D4" t="b">
         <v>1</v>

</xml_diff>